<commit_message>
add motor2 information in main page.
</commit_message>
<xml_diff>
--- a/DGUS/变量地址分配.xlsx
+++ b/DGUS/变量地址分配.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="191">
   <si>
     <t>变量名称</t>
   </si>
@@ -188,12 +188,6 @@
     <t>0x0002</t>
   </si>
   <si>
-    <t>0x0004</t>
-  </si>
-  <si>
-    <t>0x0006</t>
-  </si>
-  <si>
     <t>0x0008</t>
   </si>
   <si>
@@ -245,9 +239,6 @@
     <t>0：停止 1：运行</t>
   </si>
   <si>
-    <t>当前过程</t>
-  </si>
-  <si>
     <t>回零按钮</t>
   </si>
   <si>
@@ -407,9 +398,6 @@
     <t>返回按钮</t>
   </si>
   <si>
-    <t>累加角度（脉冲）</t>
-  </si>
-  <si>
     <t>步脉冲数 01</t>
   </si>
   <si>
@@ -576,6 +564,30 @@
   </si>
   <si>
     <t>过程一前进按钮\设置按钮</t>
+  </si>
+  <si>
+    <t>0x0001</t>
+  </si>
+  <si>
+    <t>电机1过程</t>
+  </si>
+  <si>
+    <t>电机2过程</t>
+  </si>
+  <si>
+    <t>0x0003</t>
+  </si>
+  <si>
+    <t>0x0005</t>
+  </si>
+  <si>
+    <t>0x0007</t>
+  </si>
+  <si>
+    <t>电机1角度</t>
+  </si>
+  <si>
+    <t>电机2角度</t>
   </si>
 </sst>
 </file>
@@ -995,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1025,692 +1037,714 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>183</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>184</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>185</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>186</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>189</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>187</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>190</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>188</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>186</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>182</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>129</v>
+        <v>84</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>128</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>126</v>
       </c>
       <c r="C20" t="s">
-        <v>128</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>124</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
         <v>125</v>
-      </c>
-      <c r="C22" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B24" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B25" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B32" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B33" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B34" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B35" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B36" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B40" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B41" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B42" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B43" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C43" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B44" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B45" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C45" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B46" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C46" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B47" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C47" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B48" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C48" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B49" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C49" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>171</v>
+        <v>118</v>
       </c>
       <c r="B50" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>172</v>
+        <v>119</v>
       </c>
       <c r="B51" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C51" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B52" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C52" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B53" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C53" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B54" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C54" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B55" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C55" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B56" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C56" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B57" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C57" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B58" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C58" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B59" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C59" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B60" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C60" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B61" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C61" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B62" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C62" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B63" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C63" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B64" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C64" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>180</v>
+      </c>
+      <c r="B65" t="s">
+        <v>165</v>
+      </c>
+      <c r="C65" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>181</v>
+      </c>
+      <c r="B66" t="s">
+        <v>166</v>
+      </c>
+      <c r="C66" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1734,7 +1768,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
保存eeprom ready with problem.
</commit_message>
<xml_diff>
--- a/DGUS/变量地址分配.xlsx
+++ b/DGUS/变量地址分配.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="140">
   <si>
     <t>变量名称</t>
   </si>
@@ -269,9 +269,6 @@
     <t>件数</t>
   </si>
   <si>
-    <t>花样号</t>
-  </si>
-  <si>
     <t>当前步数</t>
   </si>
   <si>
@@ -429,6 +426,15 @@
   </si>
   <si>
     <t>0x000F</t>
+  </si>
+  <si>
+    <t>0x000A</t>
+  </si>
+  <si>
+    <t>当前花样号</t>
+  </si>
+  <si>
+    <t>总花样数</t>
   </si>
 </sst>
 </file>
@@ -848,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -876,7 +882,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" t="s">
         <v>64</v>
@@ -893,7 +899,7 @@
         <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -901,183 +907,183 @@
         <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>138</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>139</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="B16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>112</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C20" t="s">
         <v>62</v>
@@ -1085,10 +1091,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
         <v>62</v>
@@ -1096,10 +1102,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C22" t="s">
         <v>62</v>
@@ -1107,10 +1113,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
         <v>62</v>
@@ -1118,10 +1124,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C24" t="s">
         <v>62</v>
@@ -1129,10 +1135,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>116</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="C25" t="s">
         <v>62</v>
@@ -1140,10 +1146,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>115</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C26" t="s">
         <v>62</v>
@@ -1151,10 +1157,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C27" t="s">
         <v>62</v>
@@ -1162,10 +1168,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C28" t="s">
         <v>62</v>
@@ -1173,10 +1179,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
         <v>62</v>
@@ -1184,10 +1190,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="B30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C30" t="s">
         <v>62</v>
@@ -1195,10 +1201,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C31" t="s">
         <v>62</v>
@@ -1206,10 +1212,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
         <v>62</v>
@@ -1217,10 +1223,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
         <v>62</v>
@@ -1228,10 +1234,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="B34" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C34" t="s">
         <v>62</v>
@@ -1239,67 +1245,78 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>121</v>
+        <v>72</v>
+      </c>
+      <c r="B35" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>123</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>124</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>127</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>